<commit_message>
Noise Removal in pipeline
</commit_message>
<xml_diff>
--- a/npec_hades_deployment/src/timeseries/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/measurements.xlsx
+++ b/npec_hades_deployment/src/timeseries/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/measurements.xlsx
@@ -476,10 +476,10 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>1968</v>
+        <v>2004</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -493,10 +493,10 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>2139</v>
+        <v>2174</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -510,7 +510,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>2272</v>
+        <v>2291</v>
       </c>
       <c r="G4" t="n">
         <v>4</v>
@@ -527,7 +527,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>1911</v>
+        <v>1972</v>
       </c>
       <c r="G5" t="n">
         <v>3</v>
@@ -544,10 +544,10 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>1333</v>
+        <v>1352</v>
       </c>
       <c r="G6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Root Measurement MM Conversion
</commit_message>
<xml_diff>
--- a/npec_hades_deployment/src/timeseries/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/measurements.xlsx
+++ b/npec_hades_deployment/src/timeseries/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/90_13_Exp32_coumarins_01_ROOT1_Fish Eye Corrected_A0/measurements.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,25 +441,40 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Primary_length(px)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Primary_length(mm)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Lateral_length(px)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Lateral_length(mm)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total_length(px)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Total_length(mm)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Leaf_size(px)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Lateral_root_count</t>
         </is>
@@ -472,13 +487,28 @@
       <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>713.7350647362948</v>
+      </c>
+      <c r="D2" t="n">
+        <v>29.3959982103616</v>
+      </c>
+      <c r="E2" t="n">
+        <v>204.509667991878</v>
+      </c>
       <c r="F2" t="n">
+        <v>8.422965511036047</v>
+      </c>
+      <c r="G2" t="n">
+        <v>918.2447327281728</v>
+      </c>
+      <c r="H2" t="n">
+        <v>37.81896372139765</v>
+      </c>
+      <c r="I2" t="n">
         <v>2004</v>
       </c>
-      <c r="G2" t="n">
+      <c r="J2" t="n">
         <v>3</v>
       </c>
     </row>
@@ -489,13 +519,28 @@
       <c r="B3" t="n">
         <v>4</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>700.9777054234141</v>
+      </c>
+      <c r="D3" t="n">
+        <v>28.8705717180133</v>
+      </c>
+      <c r="E3" t="n">
+        <v>145.2670273047587</v>
+      </c>
       <c r="F3" t="n">
+        <v>5.982989327073321</v>
+      </c>
+      <c r="G3" t="n">
+        <v>846.2447327281728</v>
+      </c>
+      <c r="H3" t="n">
+        <v>34.85356104508662</v>
+      </c>
+      <c r="I3" t="n">
         <v>2174</v>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>4</v>
       </c>
     </row>
@@ -506,13 +551,28 @@
       <c r="B4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>745.4163056034267</v>
+      </c>
+      <c r="D4" t="n">
+        <v>30.70082649447615</v>
+      </c>
+      <c r="E4" t="n">
+        <v>139.3675323681472</v>
+      </c>
       <c r="F4" t="n">
+        <v>5.740011853824552</v>
+      </c>
+      <c r="G4" t="n">
+        <v>884.7838379715739</v>
+      </c>
+      <c r="H4" t="n">
+        <v>36.4408383483007</v>
+      </c>
+      <c r="I4" t="n">
         <v>2291</v>
       </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -523,13 +583,28 @@
       <c r="B5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>656.1198410471449</v>
+      </c>
+      <c r="D5" t="n">
+        <v>27.02304906419405</v>
+      </c>
+      <c r="E5" t="n">
+        <v>12.24264068711928</v>
+      </c>
       <c r="F5" t="n">
+        <v>0.5042272147041367</v>
+      </c>
+      <c r="G5" t="n">
+        <v>668.3624817342642</v>
+      </c>
+      <c r="H5" t="n">
+        <v>27.52727627889819</v>
+      </c>
+      <c r="I5" t="n">
         <v>1972</v>
       </c>
-      <c r="G5" t="n">
+      <c r="J5" t="n">
         <v>3</v>
       </c>
     </row>
@@ -540,13 +615,28 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>223.2375900532359</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9.1942964860707</v>
+      </c>
+      <c r="E6" t="n">
+        <v>84.52691193458119</v>
+      </c>
       <c r="F6" t="n">
+        <v>3.481337928765471</v>
+      </c>
+      <c r="G6" t="n">
+        <v>307.7645019878171</v>
+      </c>
+      <c r="H6" t="n">
+        <v>12.67563441483617</v>
+      </c>
+      <c r="I6" t="n">
         <v>1352</v>
       </c>
-      <c r="G6" t="n">
+      <c r="J6" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>